<commit_message>
[Update] Joined both BOM files
</commit_message>
<xml_diff>
--- a/manuFiles/austinBom.xlsx
+++ b/manuFiles/austinBom.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="bom" sheetId="1" r:id="rId3"/>
+    <sheet state="visible" name="bom (1)" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -34,7 +34,7 @@
     <t>Manufacturer Part number</t>
   </si>
   <si>
-    <t xml:space="preserve">RI1-3, RL1-108m </t>
+    <t>RL108,RL107,RL106,RL105,RL104,RL103,RL102,RL101,RL100,RL99,RL98,RL97,RL96,RL95,RL94,RL93,RL92,RL91,RL90,RL89,RL88,RL87,RL86,RL85,RL84,RL83,RL82,RL81,RL80,RL79,RL78,RL77,RL76,RL75,RL74,RL73,RL72,RL71,RL70,RL69,RL68,RL67,RL66,RL65,RL64,RL63,RL62,RL60,RL58,RL57,RL56,RL55,RL54,RL53,RL52,RL51,RL50,RL49,RL48,RL47,RL46,RL45,RL44,RL43,RL42,RL41,RL40,RL39,RL38,RL37,RL36,RL34,RL33,RL32,RL31,RL30,RL29,RL28,RL27,RL26,RL25,RL24,RL23,RL22,RL21,RL20,RL19,RL18,RL17,RL16,RL15,RL14,RL13,RL12,RL11,RL10,RL9,RL8,RL7,RL6,RL5,RL4,RL3,RL2,RL1,RI3,RI2,RI1</t>
   </si>
   <si>
     <t>1206</t>
@@ -115,7 +115,7 @@
     <t>C282732</t>
   </si>
   <si>
-    <t>D1-108, DRST1</t>
+    <t>D1,D2,D3,D4,D5,D6,D7,D8,D9,D10,D11,D12,D20,D21,D22,D23,D24,D25,D26,D27,D28,D29,D30,D31,D40,D41,D42,D43,D44,D45,D46,D47,D48,D49,D50,D51,D61,D62,D63,D64,D65,D66,D67,D68,D69,D70,D71,D73,D79,D96,D80,D97,D81,D98,D82,D83,D84,D99,D85,D86,D87,D88,D100,D89,D101,D102,D13,D32,D52,D91,D103,D14,D33,D53,D15,D35,D54,D74,D104,D16,D36,D55,D75,D92,D105,D17,D37,D56,D76,D93,D106,D18,D38,D57,D77,D94,D107,D19,D39,D59,D95,D108,D72,D90,DRST1</t>
   </si>
   <si>
     <t>SOD-123</t>
@@ -157,7 +157,7 @@
     <t>Fuse 1.5A trip</t>
   </si>
   <si>
-    <t>C70117</t>
+    <t>C70118</t>
   </si>
   <si>
     <t>J1</t>
@@ -257,7 +257,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -265,25 +265,18 @@
     </font>
     <font>
       <b/>
+      <sz val="9.0"/>
+      <name val="Arial"/>
     </font>
-    <font/>
     <font>
-      <u/>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
+      <sz val="9.0"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="10.0"/>
+      <sz val="9.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
-      <name val="Proxima Nova"/>
     </font>
   </fonts>
   <fills count="2">
@@ -300,37 +293,25 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -347,14 +328,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.57"/>
+    <col customWidth="1" min="1" max="1" width="21.0"/>
     <col customWidth="1" min="2" max="2" width="20.86"/>
     <col customWidth="1" min="3" max="3" width="19.0"/>
     <col customWidth="1" min="4" max="4" width="14.43"/>
@@ -396,17 +377,17 @@
       <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>108.0</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -418,7 +399,7 @@
       <c r="D3" s="4">
         <v>1.0</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -429,7 +410,7 @@
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -441,14 +422,14 @@
       <c r="D4" s="4">
         <v>1.0</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -460,14 +441,14 @@
       <c r="D5" s="4">
         <v>1.0</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>21</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -479,17 +460,17 @@
       <c r="D6" s="4">
         <v>1.0</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>23</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -498,17 +479,17 @@
       <c r="D7" s="4">
         <v>3.0</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>27</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -517,17 +498,17 @@
       <c r="D8" s="4">
         <v>2.0</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>30</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -536,14 +517,14 @@
       <c r="D9" s="4">
         <v>6.0</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -552,17 +533,17 @@
       <c r="C10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>105.0</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -574,7 +555,7 @@
       <c r="D11" s="4">
         <v>1.0</v>
       </c>
-      <c r="E11" s="6" t="str">
+      <c r="E11" s="5" t="str">
         <f>HYPERLINK("https://lcsc.com/product-detail/Others_ROHM-Semicon_RB060M-60TR_ROHM-Semicon-RB060M-60TR_C114257.html","C114257")</f>
         <v>C114257</v>
       </c>
@@ -586,7 +567,7 @@
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -598,14 +579,14 @@
       <c r="D12" s="4">
         <v>1.0</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>44</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -617,14 +598,14 @@
       <c r="D13" s="4">
         <v>1.0</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -636,7 +617,7 @@
       <c r="D14" s="4">
         <v>1.0</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>52</v>
       </c>
       <c r="F14" s="4" t="s">
@@ -647,7 +628,7 @@
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="6" t="s">
         <v>54</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -659,14 +640,14 @@
       <c r="D15" s="4">
         <v>1.0</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="5" t="s">
         <v>57</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>58</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -678,14 +659,14 @@
       <c r="D16" s="4">
         <v>1.0</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="5" t="s">
         <v>61</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>62</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -697,14 +678,14 @@
       <c r="D17" s="4">
         <v>1.0</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="5" t="s">
         <v>64</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>65</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -716,14 +697,14 @@
       <c r="D18" s="4">
         <v>1.0</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="5" t="s">
         <v>67</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="6" t="s">
         <v>68</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -735,7 +716,7 @@
       <c r="D19" s="4">
         <v>1.0</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="5" t="s">
         <v>71</v>
       </c>
       <c r="F19" s="4" t="s">
@@ -746,7 +727,7 @@
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="6" t="s">
         <v>73</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -758,7 +739,7 @@
       <c r="D20" s="4">
         <v>1.0</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="5" t="s">
         <v>75</v>
       </c>
       <c r="F20" s="4" t="s">
@@ -769,7 +750,7 @@
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="6" t="s">
         <v>77</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -781,7 +762,7 @@
       <c r="D21" s="4">
         <v>1.0</v>
       </c>
-      <c r="E21" s="6" t="str">
+      <c r="E21" s="5" t="str">
         <f>HYPERLINK("https://lcsc.com/product-detail/Diodes-ESD_STMicroelectronics_USBLC6-2SC6_USBLC6-2SC6_C7519.html","C7519")</f>
         <v>C7519</v>
       </c>
@@ -813,6 +794,9 @@
     <hyperlink r:id="rId17" ref="E19"/>
     <hyperlink r:id="rId18" ref="E20"/>
   </hyperlinks>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="landscape"/>
   <drawing r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>